<commit_message>
Mas avances de consumo de APIs
</commit_message>
<xml_diff>
--- a/Doc/API resources.xlsx
+++ b/Doc/API resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacat\OneDrive\Documentos\irune-api-consumption\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F10D3C-D23F-4BE5-9C3E-81D9208C821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A631704-323A-4275-9FDC-6412D0E2D545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{C512B82E-D8CB-4BE0-A2B7-61539175D884}"/>
   </bookViews>
@@ -125,9 +125,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -443,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCF55C2-BBA9-4A3F-8E1E-820E86E60CB7}">
-  <dimension ref="A3:E5"/>
+  <dimension ref="A3:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +510,9 @@
         <v>10</v>
       </c>
     </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{158BC4D9-7C35-480C-ABC0-9DBF2BD31617}"/>

</xml_diff>